<commit_message>
Se cambia paradigma se trabaja con postgre
</commit_message>
<xml_diff>
--- a/MARCA X PROVEEDOR.xlsx
+++ b/MARCA X PROVEEDOR.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOSTRADOR 4\Desktop\Archivo\Tareas wismi\Prototipo MarkForge\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="PDqTixisKWRwDjOFXm1Z8T/volc3Kw5XBaese8HMnLI="/>
@@ -1245,34 +1253,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Abril Fatface"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Abril Fatface"/>
     </font>
@@ -1282,7 +1290,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1298,7 +1306,13 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -1312,6 +1326,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1324,6 +1339,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1336,6 +1352,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -1350,75 +1367,73 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF00B050"/>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1608,64 +1623,65 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:CH1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="14.86"/>
-    <col customWidth="1" min="4" max="4" width="23.29"/>
-    <col customWidth="1" min="5" max="5" width="21.57"/>
-    <col customWidth="1" min="6" max="6" width="19.14"/>
-    <col customWidth="1" min="7" max="7" width="24.71"/>
-    <col customWidth="1" min="8" max="8" width="21.29"/>
-    <col customWidth="1" min="9" max="9" width="13.86"/>
-    <col customWidth="1" min="10" max="10" width="14.0"/>
-    <col customWidth="1" min="11" max="11" width="12.29"/>
-    <col customWidth="1" min="12" max="12" width="26.86"/>
-    <col customWidth="1" min="13" max="13" width="20.43"/>
-    <col customWidth="1" min="14" max="19" width="10.71"/>
-    <col customWidth="1" min="20" max="20" width="19.14"/>
-    <col customWidth="1" min="21" max="21" width="19.43"/>
-    <col customWidth="1" min="22" max="22" width="27.14"/>
-    <col customWidth="1" min="23" max="23" width="17.57"/>
-    <col customWidth="1" min="24" max="24" width="18.0"/>
-    <col customWidth="1" min="25" max="27" width="10.71"/>
-    <col customWidth="1" min="28" max="28" width="16.0"/>
-    <col customWidth="1" min="29" max="30" width="10.71"/>
-    <col customWidth="1" min="31" max="31" width="8.0"/>
-    <col customWidth="1" min="32" max="35" width="10.71"/>
-    <col customWidth="1" min="36" max="37" width="12.0"/>
-    <col customWidth="1" min="38" max="56" width="10.71"/>
-    <col customWidth="1" min="57" max="57" width="18.14"/>
-    <col customWidth="1" min="58" max="64" width="10.71"/>
-    <col customWidth="1" min="65" max="65" width="28.57"/>
-    <col customWidth="1" min="66" max="66" width="21.57"/>
-    <col customWidth="1" min="67" max="67" width="18.57"/>
-    <col customWidth="1" min="68" max="68" width="37.57"/>
-    <col customWidth="1" min="69" max="73" width="10.71"/>
-    <col customWidth="1" min="74" max="74" width="16.43"/>
-    <col customWidth="1" min="75" max="78" width="10.71"/>
-    <col customWidth="1" min="79" max="79" width="14.14"/>
-    <col customWidth="1" min="80" max="86" width="10.71"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+    <col min="14" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" customWidth="1"/>
+    <col min="22" max="22" width="27.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
+    <col min="25" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="30" width="10.7109375" customWidth="1"/>
+    <col min="31" max="31" width="8" customWidth="1"/>
+    <col min="32" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="37" width="12" customWidth="1"/>
+    <col min="38" max="56" width="10.7109375" customWidth="1"/>
+    <col min="57" max="57" width="18.140625" customWidth="1"/>
+    <col min="58" max="64" width="10.7109375" customWidth="1"/>
+    <col min="65" max="65" width="28.5703125" customWidth="1"/>
+    <col min="66" max="66" width="21.5703125" customWidth="1"/>
+    <col min="67" max="67" width="18.5703125" customWidth="1"/>
+    <col min="68" max="68" width="37.5703125" customWidth="1"/>
+    <col min="69" max="73" width="10.7109375" customWidth="1"/>
+    <col min="74" max="74" width="16.42578125" customWidth="1"/>
+    <col min="75" max="78" width="10.7109375" customWidth="1"/>
+    <col min="79" max="79" width="14.140625" customWidth="1"/>
+    <col min="80" max="86" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:86">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,7 +1941,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:86">
       <c r="A2" s="4" t="s">
         <v>86</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:86">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
@@ -2355,7 +2371,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:86">
       <c r="A4" s="4" t="s">
         <v>91</v>
       </c>
@@ -2569,7 +2585,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:86">
       <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
@@ -2781,7 +2797,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:86">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -2993,7 +3009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:86">
       <c r="A7" s="4" t="s">
         <v>94</v>
       </c>
@@ -3207,7 +3223,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:86">
       <c r="A8" s="4" t="s">
         <v>95</v>
       </c>
@@ -3421,7 +3437,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:86">
       <c r="A9" s="4" t="s">
         <v>96</v>
       </c>
@@ -3633,7 +3649,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:86">
       <c r="A10" s="4" t="s">
         <v>97</v>
       </c>
@@ -3845,7 +3861,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:86">
       <c r="A11" s="4" t="s">
         <v>98</v>
       </c>
@@ -4057,7 +4073,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:86">
       <c r="A12" s="4" t="s">
         <v>99</v>
       </c>
@@ -4271,7 +4287,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:86">
       <c r="A13" s="4" t="s">
         <v>100</v>
       </c>
@@ -4483,7 +4499,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:86">
       <c r="A14" s="4" t="s">
         <v>101</v>
       </c>
@@ -4695,7 +4711,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:86">
       <c r="A15" s="4" t="s">
         <v>102</v>
       </c>
@@ -4907,7 +4923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:86">
       <c r="A16" s="4" t="s">
         <v>103</v>
       </c>
@@ -5119,7 +5135,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:86">
       <c r="A17" s="4" t="s">
         <v>104</v>
       </c>
@@ -5331,7 +5347,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:86">
       <c r="A18" s="4" t="s">
         <v>105</v>
       </c>
@@ -5543,7 +5559,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:86">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -5755,7 +5771,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:86">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -5967,7 +5983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:86" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>108</v>
       </c>
@@ -6179,7 +6195,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:86" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>109</v>
       </c>
@@ -6391,7 +6407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:86" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>110</v>
       </c>
@@ -6603,7 +6619,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:86" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>111</v>
       </c>
@@ -6815,7 +6831,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:86" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>112</v>
       </c>
@@ -7027,7 +7043,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:86" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>113</v>
       </c>
@@ -7239,7 +7255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:86" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>114</v>
       </c>
@@ -7449,7 +7465,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:86" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>115</v>
       </c>
@@ -7661,7 +7677,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:86" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
@@ -7871,7 +7887,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:86" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>117</v>
       </c>
@@ -8081,7 +8097,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:86" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>118</v>
       </c>
@@ -8291,7 +8307,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:86" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>119</v>
       </c>
@@ -8501,7 +8517,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:86" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>120</v>
       </c>
@@ -8713,7 +8729,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:86" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>121</v>
       </c>
@@ -8923,7 +8939,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:86" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>122</v>
       </c>
@@ -9133,7 +9149,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:86" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>123</v>
       </c>
@@ -9343,7 +9359,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:86" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>124</v>
       </c>
@@ -9555,7 +9571,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:86" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>125</v>
       </c>
@@ -9769,7 +9785,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:86" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>126</v>
       </c>
@@ -9981,7 +9997,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:86" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>127</v>
       </c>
@@ -10193,7 +10209,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:86" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>128</v>
       </c>
@@ -10411,7 +10427,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:86" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>129</v>
       </c>
@@ -10621,7 +10637,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:86" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>130</v>
       </c>
@@ -10831,7 +10847,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:86" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>131</v>
       </c>
@@ -11043,7 +11059,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:86" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>132</v>
       </c>
@@ -11253,7 +11269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:86" ht="15.75" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>133</v>
       </c>
@@ -11465,7 +11481,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:86" ht="15.75" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>134</v>
       </c>
@@ -11677,7 +11693,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:86" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>135</v>
       </c>
@@ -11889,7 +11905,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:86" ht="15.75" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>136</v>
       </c>
@@ -12101,7 +12117,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:86" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>137</v>
       </c>
@@ -12313,7 +12329,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:86" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>138</v>
       </c>
@@ -12525,7 +12541,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:86" ht="15.75" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>139</v>
       </c>
@@ -12737,7 +12753,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:86" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>140</v>
       </c>
@@ -12949,7 +12965,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:86" ht="15.75" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>141</v>
       </c>
@@ -13161,7 +13177,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:86" ht="15.75" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>142</v>
       </c>
@@ -13373,7 +13389,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:86" ht="15.75" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>143</v>
       </c>
@@ -13585,7 +13601,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:86" ht="15.75" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>144</v>
       </c>
@@ -13797,7 +13813,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:86" ht="15.75" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>145</v>
       </c>
@@ -14011,7 +14027,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:86" ht="15.75" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>146</v>
       </c>
@@ -14223,7 +14239,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:86" ht="15.75" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>147</v>
       </c>
@@ -14435,7 +14451,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:86" ht="15.75" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>148</v>
       </c>
@@ -14647,7 +14663,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:86" ht="15.75" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>149</v>
       </c>
@@ -14859,7 +14875,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:86" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>150</v>
       </c>
@@ -15071,7 +15087,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:86" ht="15.75" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>151</v>
       </c>
@@ -15283,7 +15299,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:86" ht="15.75" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>152</v>
       </c>
@@ -15495,7 +15511,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:86" ht="15.75" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>153</v>
       </c>
@@ -15705,7 +15721,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:86" ht="15.75" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>154</v>
       </c>
@@ -15915,7 +15931,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:86" ht="15.75" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>155</v>
       </c>
@@ -16125,7 +16141,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:86" ht="15.75" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>156</v>
       </c>
@@ -16335,7 +16351,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:86" ht="15.75" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>157</v>
       </c>
@@ -16547,7 +16563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:86" ht="15.75" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>158</v>
       </c>
@@ -16761,7 +16777,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:86" ht="15.75" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>159</v>
       </c>
@@ -16971,7 +16987,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:86" ht="15.75" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>160</v>
       </c>
@@ -17185,7 +17201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:86" ht="15.75" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>161</v>
       </c>
@@ -17399,7 +17415,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:86" ht="15.75" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>162</v>
       </c>
@@ -17609,7 +17625,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:86" ht="15.75" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>163</v>
       </c>
@@ -17819,7 +17835,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:86" ht="15.75" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>164</v>
       </c>
@@ -18035,7 +18051,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:86" ht="15.75" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
@@ -18245,7 +18261,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:86" ht="15.75" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>166</v>
       </c>
@@ -18455,7 +18471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:86" ht="15.75" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>167</v>
       </c>
@@ -18665,7 +18681,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:86" ht="15.75" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>168</v>
       </c>
@@ -18875,7 +18891,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:86" ht="15.75" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>169</v>
       </c>
@@ -19087,7 +19103,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:86" ht="15.75" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>170</v>
       </c>
@@ -19297,7 +19313,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:86" ht="15.75" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>171</v>
       </c>
@@ -19507,7 +19523,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:86" ht="15.75" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>172</v>
       </c>
@@ -19721,7 +19737,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:86" ht="15.75" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>173</v>
       </c>
@@ -19933,7 +19949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:86" ht="15.75" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>174</v>
       </c>
@@ -20143,7 +20159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:86" ht="15.75" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>175</v>
       </c>
@@ -20357,7 +20373,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:86" ht="15.75" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>176</v>
       </c>
@@ -20567,7 +20583,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:86" ht="15.75" customHeight="1">
       <c r="A90" s="4" t="s">
         <v>177</v>
       </c>
@@ -20777,7 +20793,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:86" ht="15.75" customHeight="1">
       <c r="A91" s="4" t="s">
         <v>178</v>
       </c>
@@ -20985,7 +21001,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:86" ht="15.75" customHeight="1">
       <c r="A92" s="4" t="s">
         <v>179</v>
       </c>
@@ -21197,7 +21213,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:86" ht="15.75" customHeight="1">
       <c r="A93" s="4" t="s">
         <v>180</v>
       </c>
@@ -21409,7 +21425,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:86" ht="15.75" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>181</v>
       </c>
@@ -21619,7 +21635,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:86" ht="15.75" customHeight="1">
       <c r="A95" s="4" t="s">
         <v>182</v>
       </c>
@@ -21829,7 +21845,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:86" ht="15.75" customHeight="1">
       <c r="A96" s="4" t="s">
         <v>183</v>
       </c>
@@ -22039,7 +22055,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:86" ht="15.75" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>184</v>
       </c>
@@ -22249,7 +22265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:86" ht="15.75" customHeight="1">
       <c r="A98" s="4" t="s">
         <v>185</v>
       </c>
@@ -22461,7 +22477,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:86" ht="15.75" customHeight="1">
       <c r="A99" s="4" t="s">
         <v>186</v>
       </c>
@@ -22673,7 +22689,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:86" ht="15.75" customHeight="1">
       <c r="A100" s="4" t="s">
         <v>187</v>
       </c>
@@ -22883,7 +22899,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:86" ht="15.75" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>188</v>
       </c>
@@ -23097,7 +23113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:86" ht="15.75" customHeight="1">
       <c r="A102" s="4" t="s">
         <v>189</v>
       </c>
@@ -23309,7 +23325,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:86" ht="15.75" customHeight="1">
       <c r="A103" s="4" t="s">
         <v>190</v>
       </c>
@@ -23519,7 +23535,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:86" ht="15.75" customHeight="1">
       <c r="A104" s="4" t="s">
         <v>191</v>
       </c>
@@ -23729,7 +23745,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:86" ht="15.75" customHeight="1">
       <c r="A105" s="4" t="s">
         <v>192</v>
       </c>
@@ -23939,7 +23955,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:86" ht="15.75" customHeight="1">
       <c r="A106" s="4" t="s">
         <v>193</v>
       </c>
@@ -24151,7 +24167,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:86" ht="15.75" customHeight="1">
       <c r="A107" s="4" t="s">
         <v>194</v>
       </c>
@@ -24363,7 +24379,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:86" ht="15.75" customHeight="1">
       <c r="A108" s="4" t="s">
         <v>195</v>
       </c>
@@ -24575,7 +24591,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:86" ht="15.75" customHeight="1">
       <c r="A109" s="4" t="s">
         <v>196</v>
       </c>
@@ -24787,7 +24803,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:86" ht="15.75" customHeight="1">
       <c r="A110" s="4" t="s">
         <v>197</v>
       </c>
@@ -24997,7 +25013,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:86" ht="15.75" customHeight="1">
       <c r="A111" s="4" t="s">
         <v>198</v>
       </c>
@@ -25209,7 +25225,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:86" ht="15.75" customHeight="1">
       <c r="A112" s="4" t="s">
         <v>199</v>
       </c>
@@ -25419,7 +25435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:86" ht="15.75" customHeight="1">
       <c r="A113" s="4" t="s">
         <v>200</v>
       </c>
@@ -25629,7 +25645,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:86" ht="15.75" customHeight="1">
       <c r="A114" s="4" t="s">
         <v>201</v>
       </c>
@@ -25843,7 +25859,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:86" ht="15.75" customHeight="1">
       <c r="A115" s="4" t="s">
         <v>202</v>
       </c>
@@ -26053,7 +26069,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:86" ht="15.75" customHeight="1">
       <c r="A116" s="4" t="s">
         <v>203</v>
       </c>
@@ -26263,7 +26279,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:86" ht="15.75" customHeight="1">
       <c r="A117" s="4" t="s">
         <v>204</v>
       </c>
@@ -26473,7 +26489,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:86" ht="15.75" customHeight="1">
       <c r="A118" s="4" t="s">
         <v>205</v>
       </c>
@@ -26683,7 +26699,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:86" ht="15.75" customHeight="1">
       <c r="A119" s="4" t="s">
         <v>206</v>
       </c>
@@ -26899,7 +26915,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:86" ht="15.75" customHeight="1">
       <c r="A120" s="4" t="s">
         <v>207</v>
       </c>
@@ -27115,7 +27131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:86" ht="15.75" customHeight="1">
       <c r="A121" s="4" t="s">
         <v>208</v>
       </c>
@@ -27329,7 +27345,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:86" ht="15.75" customHeight="1">
       <c r="A122" s="4" t="s">
         <v>209</v>
       </c>
@@ -27543,7 +27559,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:86" ht="15.75" customHeight="1">
       <c r="A123" s="4" t="s">
         <v>210</v>
       </c>
@@ -27753,7 +27769,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:86" ht="15.75" customHeight="1">
       <c r="A124" s="4" t="s">
         <v>211</v>
       </c>
@@ -27967,7 +27983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:86" ht="15.75" customHeight="1">
       <c r="A125" s="4" t="s">
         <v>212</v>
       </c>
@@ -28179,7 +28195,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:86" ht="15.75" customHeight="1">
       <c r="A126" s="4" t="s">
         <v>213</v>
       </c>
@@ -28389,7 +28405,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:86" ht="15.75" customHeight="1">
       <c r="A127" s="4" t="s">
         <v>214</v>
       </c>
@@ -28599,7 +28615,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:86" ht="15.75" customHeight="1">
       <c r="A128" s="4" t="s">
         <v>215</v>
       </c>
@@ -28809,7 +28825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:86" ht="15.75" customHeight="1">
       <c r="A129" s="4" t="s">
         <v>216</v>
       </c>
@@ -29019,7 +29035,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:86" ht="15.75" customHeight="1">
       <c r="A130" s="4" t="s">
         <v>217</v>
       </c>
@@ -29229,7 +29245,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:86" ht="15.75" customHeight="1">
       <c r="A131" s="4" t="s">
         <v>218</v>
       </c>
@@ -29439,7 +29455,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:86" ht="15.75" customHeight="1">
       <c r="A132" s="4" t="s">
         <v>219</v>
       </c>
@@ -29649,7 +29665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:86" ht="15.75" customHeight="1">
       <c r="A133" s="4" t="s">
         <v>220</v>
       </c>
@@ -29859,7 +29875,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:86" ht="15.75" customHeight="1">
       <c r="A134" s="4" t="s">
         <v>221</v>
       </c>
@@ -30069,7 +30085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:86" ht="15.75" customHeight="1">
       <c r="A135" s="4" t="s">
         <v>222</v>
       </c>
@@ -30279,7 +30295,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:86" ht="15.75" customHeight="1">
       <c r="A136" s="4" t="s">
         <v>223</v>
       </c>
@@ -30489,7 +30505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:86" ht="15.75" customHeight="1">
       <c r="A137" s="4" t="s">
         <v>224</v>
       </c>
@@ -30699,7 +30715,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:86" ht="15.75" customHeight="1">
       <c r="A138" s="4" t="s">
         <v>225</v>
       </c>
@@ -30911,7 +30927,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:86" ht="15.75" customHeight="1">
       <c r="A139" s="4" t="s">
         <v>226</v>
       </c>
@@ -31123,7 +31139,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:86" ht="15.75" customHeight="1">
       <c r="A140" s="4" t="s">
         <v>227</v>
       </c>
@@ -31337,7 +31353,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:86" ht="15.75" customHeight="1">
       <c r="A141" s="4" t="s">
         <v>228</v>
       </c>
@@ -31547,7 +31563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:86" ht="15.75" customHeight="1">
       <c r="A142" s="4" t="s">
         <v>229</v>
       </c>
@@ -31757,7 +31773,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:86" ht="15.75" customHeight="1">
       <c r="A143" s="4" t="s">
         <v>230</v>
       </c>
@@ -31967,7 +31983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:86" ht="15.75" customHeight="1">
       <c r="A144" s="4" t="s">
         <v>231</v>
       </c>
@@ -32177,7 +32193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:86" ht="15.75" customHeight="1">
       <c r="A145" s="4" t="s">
         <v>232</v>
       </c>
@@ -32387,7 +32403,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:86" ht="15.75" customHeight="1">
       <c r="A146" s="4" t="s">
         <v>233</v>
       </c>
@@ -32597,7 +32613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:86" ht="15.75" customHeight="1">
       <c r="A147" s="4" t="s">
         <v>234</v>
       </c>
@@ -32807,7 +32823,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:86" ht="15.75" customHeight="1">
       <c r="A148" s="4" t="s">
         <v>235</v>
       </c>
@@ -33017,7 +33033,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:86" ht="15.75" customHeight="1">
       <c r="A149" s="4" t="s">
         <v>236</v>
       </c>
@@ -33227,7 +33243,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:86" ht="15.75" customHeight="1">
       <c r="A150" s="4" t="s">
         <v>237</v>
       </c>
@@ -33437,7 +33453,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:86" ht="15.75" customHeight="1">
       <c r="A151" s="4" t="s">
         <v>238</v>
       </c>
@@ -33649,7 +33665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:86" ht="15.75" customHeight="1">
       <c r="A152" s="4" t="s">
         <v>239</v>
       </c>
@@ -33863,7 +33879,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:86" ht="15.75" customHeight="1">
       <c r="A153" s="4" t="s">
         <v>240</v>
       </c>
@@ -34073,7 +34089,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:86" ht="15.75" customHeight="1">
       <c r="A154" s="4" t="s">
         <v>241</v>
       </c>
@@ -34283,7 +34299,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:86" ht="15.75" customHeight="1">
       <c r="A155" s="4" t="s">
         <v>242</v>
       </c>
@@ -34497,7 +34513,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:86" ht="15.75" customHeight="1">
       <c r="A156" s="4" t="s">
         <v>243</v>
       </c>
@@ -34707,7 +34723,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:86" ht="15.75" customHeight="1">
       <c r="A157" s="4" t="s">
         <v>244</v>
       </c>
@@ -34915,7 +34931,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:86" ht="15.75" customHeight="1">
       <c r="A158" s="4" t="s">
         <v>245</v>
       </c>
@@ -35129,7 +35145,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:86" ht="15.75" customHeight="1">
       <c r="A159" s="4" t="s">
         <v>246</v>
       </c>
@@ -35339,7 +35355,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:86" ht="15.75" customHeight="1">
       <c r="A160" s="4" t="s">
         <v>247</v>
       </c>
@@ -35553,7 +35569,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:86" ht="15.75" customHeight="1">
       <c r="A161" s="4" t="s">
         <v>248</v>
       </c>
@@ -35763,7 +35779,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:86" ht="15.75" customHeight="1">
       <c r="A162" s="4" t="s">
         <v>249</v>
       </c>
@@ -35977,7 +35993,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:86" ht="15.75" customHeight="1">
       <c r="A163" s="4" t="s">
         <v>250</v>
       </c>
@@ -36187,7 +36203,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:86" ht="15.75" customHeight="1">
       <c r="A164" s="4" t="s">
         <v>251</v>
       </c>
@@ -36397,7 +36413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:86" ht="15.75" customHeight="1">
       <c r="A165" s="4" t="s">
         <v>252</v>
       </c>
@@ -36607,7 +36623,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:86" ht="15.75" customHeight="1">
       <c r="A166" s="4" t="s">
         <v>253</v>
       </c>
@@ -36823,7 +36839,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:86" ht="15.75" customHeight="1">
       <c r="A167" s="4" t="s">
         <v>254</v>
       </c>
@@ -37033,7 +37049,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:86" ht="15.75" customHeight="1">
       <c r="A168" s="4" t="s">
         <v>255</v>
       </c>
@@ -37245,7 +37261,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:86" ht="15.75" customHeight="1">
       <c r="A169" s="4" t="s">
         <v>256</v>
       </c>
@@ -37459,7 +37475,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:86" ht="15.75" customHeight="1">
       <c r="A170" s="4" t="s">
         <v>257</v>
       </c>
@@ -37671,7 +37687,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:86" ht="15.75" customHeight="1">
       <c r="A171" s="4" t="s">
         <v>258</v>
       </c>
@@ -37881,7 +37897,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:86" ht="15.75" customHeight="1">
       <c r="A172" s="4" t="s">
         <v>259</v>
       </c>
@@ -38097,7 +38113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:86" ht="15.75" customHeight="1">
       <c r="A173" s="4" t="s">
         <v>260</v>
       </c>
@@ -38309,7 +38325,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:86" ht="15.75" customHeight="1">
       <c r="A174" s="4" t="s">
         <v>261</v>
       </c>
@@ -38521,7 +38537,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:86" ht="15.75" customHeight="1">
       <c r="A175" s="4" t="s">
         <v>262</v>
       </c>
@@ -38731,7 +38747,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:86" ht="15.75" customHeight="1">
       <c r="A176" s="4" t="s">
         <v>263</v>
       </c>
@@ -38941,7 +38957,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:86" ht="15.75" customHeight="1">
       <c r="A177" s="4" t="s">
         <v>264</v>
       </c>
@@ -39155,7 +39171,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:86" ht="15.75" customHeight="1">
       <c r="A178" s="4" t="s">
         <v>265</v>
       </c>
@@ -39369,7 +39385,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:86" ht="15.75" customHeight="1">
       <c r="A179" s="4" t="s">
         <v>266</v>
       </c>
@@ -39579,7 +39595,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:86" ht="15.75" customHeight="1">
       <c r="A180" s="4" t="s">
         <v>267</v>
       </c>
@@ -39791,7 +39807,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:86" ht="15.75" customHeight="1">
       <c r="A181" s="4" t="s">
         <v>268</v>
       </c>
@@ -40003,7 +40019,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:86" ht="15.75" customHeight="1">
       <c r="A182" s="4" t="s">
         <v>269</v>
       </c>
@@ -40219,7 +40235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:86" ht="15.75" customHeight="1">
       <c r="A183" s="4" t="s">
         <v>270</v>
       </c>
@@ -40431,7 +40447,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:86" ht="15.75" customHeight="1">
       <c r="A184" s="4" t="s">
         <v>271</v>
       </c>
@@ -40643,7 +40659,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:86" ht="15.75" customHeight="1">
       <c r="A185" s="4" t="s">
         <v>272</v>
       </c>
@@ -40853,7 +40869,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:86" ht="15.75" customHeight="1">
       <c r="A186" s="4" t="s">
         <v>273</v>
       </c>
@@ -41067,7 +41083,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:86" ht="15.75" customHeight="1">
       <c r="A187" s="4" t="s">
         <v>274</v>
       </c>
@@ -41277,7 +41293,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:86" ht="15.75" customHeight="1">
       <c r="A188" s="4" t="s">
         <v>275</v>
       </c>
@@ -41487,7 +41503,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:86" ht="15.75" customHeight="1">
       <c r="A189" s="4" t="s">
         <v>276</v>
       </c>
@@ -41697,7 +41713,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:86" ht="15.75" customHeight="1">
       <c r="A190" s="4" t="s">
         <v>277</v>
       </c>
@@ -41909,7 +41925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:86" ht="15.75" customHeight="1">
       <c r="A191" s="4" t="s">
         <v>278</v>
       </c>
@@ -42119,7 +42135,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:86" ht="15.75" customHeight="1">
       <c r="A192" s="4" t="s">
         <v>279</v>
       </c>
@@ -42333,7 +42349,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:86" ht="15.75" customHeight="1">
       <c r="A193" s="4" t="s">
         <v>280</v>
       </c>
@@ -42543,7 +42559,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:86" ht="15.75" customHeight="1">
       <c r="A194" s="4" t="s">
         <v>281</v>
       </c>
@@ -42753,7 +42769,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:86" ht="15.75" customHeight="1">
       <c r="A195" s="4" t="s">
         <v>282</v>
       </c>
@@ -42963,7 +42979,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:86" ht="15.75" customHeight="1">
       <c r="A196" s="4" t="s">
         <v>283</v>
       </c>
@@ -43173,7 +43189,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:86" ht="15.75" customHeight="1">
       <c r="A197" s="4" t="s">
         <v>284</v>
       </c>
@@ -43387,7 +43403,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:86" ht="15.75" customHeight="1">
       <c r="A198" s="4" t="s">
         <v>285</v>
       </c>
@@ -43597,7 +43613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:86" ht="15.75" customHeight="1">
       <c r="A199" s="4" t="s">
         <v>286</v>
       </c>
@@ -43809,7 +43825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:86" ht="15.75" customHeight="1">
       <c r="A200" s="4" t="s">
         <v>287</v>
       </c>
@@ -44019,7 +44035,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:86" ht="15.75" customHeight="1">
       <c r="A201" s="4" t="s">
         <v>288</v>
       </c>
@@ -44231,7 +44247,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:86" ht="15.75" customHeight="1">
       <c r="A202" s="4" t="s">
         <v>289</v>
       </c>
@@ -44443,7 +44459,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:86" ht="15.75" customHeight="1">
       <c r="A203" s="4" t="s">
         <v>290</v>
       </c>
@@ -44653,7 +44669,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:86" ht="15.75" customHeight="1">
       <c r="A204" s="4" t="s">
         <v>291</v>
       </c>
@@ -44867,7 +44883,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:86" ht="15.75" customHeight="1">
       <c r="A205" s="4" t="s">
         <v>292</v>
       </c>
@@ -45079,7 +45095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:86" ht="15.75" customHeight="1">
       <c r="A206" s="4" t="s">
         <v>293</v>
       </c>
@@ -45293,7 +45309,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:86" ht="15.75" customHeight="1">
       <c r="A207" s="4" t="s">
         <v>294</v>
       </c>
@@ -45505,7 +45521,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:86" ht="15.75" customHeight="1">
       <c r="A208" s="4" t="s">
         <v>295</v>
       </c>
@@ -45715,7 +45731,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:86" ht="15.75" customHeight="1">
       <c r="A209" s="4" t="s">
         <v>296</v>
       </c>
@@ -45925,7 +45941,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:86" ht="15.75" customHeight="1">
       <c r="A210" s="4" t="s">
         <v>297</v>
       </c>
@@ -46141,7 +46157,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:86" ht="15.75" customHeight="1">
       <c r="A211" s="4" t="s">
         <v>298</v>
       </c>
@@ -46353,7 +46369,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:86" ht="15.75" customHeight="1">
       <c r="A212" s="4" t="s">
         <v>299</v>
       </c>
@@ -46567,7 +46583,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:86" ht="15.75" customHeight="1">
       <c r="A213" s="4" t="s">
         <v>300</v>
       </c>
@@ -46777,7 +46793,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:86" ht="15.75" customHeight="1">
       <c r="A214" s="4" t="s">
         <v>301</v>
       </c>
@@ -46989,7 +47005,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:86" ht="15.75" customHeight="1">
       <c r="A215" s="4" t="s">
         <v>302</v>
       </c>
@@ -47201,7 +47217,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:86" ht="15.75" customHeight="1">
       <c r="A216" s="4" t="s">
         <v>303</v>
       </c>
@@ -47415,7 +47431,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:86" ht="15.75" customHeight="1">
       <c r="A217" s="4" t="s">
         <v>304</v>
       </c>
@@ -47631,7 +47647,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:86" ht="15.75" customHeight="1">
       <c r="A218" s="4" t="s">
         <v>305</v>
       </c>
@@ -47843,7 +47859,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:86" ht="15.75" customHeight="1">
       <c r="A219" s="4" t="s">
         <v>306</v>
       </c>
@@ -48053,7 +48069,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:86" ht="15.75" customHeight="1">
       <c r="A220" s="4" t="s">
         <v>307</v>
       </c>
@@ -48263,7 +48279,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="1:86" ht="15.75" customHeight="1">
       <c r="A221" s="4" t="s">
         <v>308</v>
       </c>
@@ -48473,7 +48489,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="222" ht="15.75" customHeight="1">
+    <row r="222" spans="1:86" ht="15.75" customHeight="1">
       <c r="A222" s="4" t="s">
         <v>309</v>
       </c>
@@ -48683,7 +48699,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="1:86" ht="15.75" customHeight="1">
       <c r="A223" s="4" t="s">
         <v>310</v>
       </c>
@@ -48893,7 +48909,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="1:86" ht="15.75" customHeight="1">
       <c r="A224" s="4" t="s">
         <v>311</v>
       </c>
@@ -49107,7 +49123,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="1:86" ht="15.75" customHeight="1">
       <c r="A225" s="4" t="s">
         <v>312</v>
       </c>
@@ -49317,7 +49333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="226" ht="15.75" customHeight="1">
+    <row r="226" spans="1:86" ht="15.75" customHeight="1">
       <c r="A226" s="4" t="s">
         <v>313</v>
       </c>
@@ -49527,7 +49543,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="1:86" ht="15.75" customHeight="1">
       <c r="A227" s="4" t="s">
         <v>314</v>
       </c>
@@ -49739,7 +49755,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="1:86" ht="15.75" customHeight="1">
       <c r="A228" s="4" t="s">
         <v>315</v>
       </c>
@@ -49949,7 +49965,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="1:86" ht="15.75" customHeight="1">
       <c r="A229" s="4" t="s">
         <v>316</v>
       </c>
@@ -50159,7 +50175,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
+    <row r="230" spans="1:86" ht="15.75" customHeight="1">
       <c r="A230" s="4" t="s">
         <v>317</v>
       </c>
@@ -50373,7 +50389,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="1:86" ht="15.75" customHeight="1">
       <c r="A231" s="4" t="s">
         <v>318</v>
       </c>
@@ -50587,7 +50603,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="1:86" ht="15.75" customHeight="1">
       <c r="A232" s="4" t="s">
         <v>319</v>
       </c>
@@ -50801,7 +50817,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="1:86" ht="15.75" customHeight="1">
       <c r="A233" s="4" t="s">
         <v>320</v>
       </c>
@@ -51015,7 +51031,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="1:86" ht="15.75" customHeight="1">
       <c r="A234" s="4" t="s">
         <v>321</v>
       </c>
@@ -51229,7 +51245,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" spans="1:86" ht="15.75" customHeight="1">
       <c r="A235" s="4" t="s">
         <v>34</v>
       </c>
@@ -51439,7 +51455,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="1:86" ht="15.75" customHeight="1">
       <c r="A236" s="4" t="s">
         <v>322</v>
       </c>
@@ -51649,7 +51665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="1:86" ht="15.75" customHeight="1">
       <c r="A237" s="4" t="s">
         <v>323</v>
       </c>
@@ -51859,7 +51875,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" spans="1:86" ht="15.75" customHeight="1">
       <c r="A238" s="4" t="s">
         <v>324</v>
       </c>
@@ -52069,7 +52085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" spans="1:86" ht="15.75" customHeight="1">
       <c r="A239" s="4" t="s">
         <v>325</v>
       </c>
@@ -52279,7 +52295,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" spans="1:86" ht="15.75" customHeight="1">
       <c r="A240" s="4" t="s">
         <v>326</v>
       </c>
@@ -52489,7 +52505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" spans="1:86" ht="15.75" customHeight="1">
       <c r="A241" s="4" t="s">
         <v>327</v>
       </c>
@@ -52701,7 +52717,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" spans="1:86" ht="15.75" customHeight="1">
       <c r="A242" s="4" t="s">
         <v>328</v>
       </c>
@@ -52913,7 +52929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" spans="1:86" ht="15.75" customHeight="1">
       <c r="A243" s="4" t="s">
         <v>329</v>
       </c>
@@ -53125,7 +53141,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="244" ht="15.75" customHeight="1">
+    <row r="244" spans="1:86" ht="15.75" customHeight="1">
       <c r="A244" s="4" t="s">
         <v>330</v>
       </c>
@@ -53337,7 +53353,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="245" ht="15.75" customHeight="1">
+    <row r="245" spans="1:86" ht="15.75" customHeight="1">
       <c r="A245" s="4" t="s">
         <v>331</v>
       </c>
@@ -53549,7 +53565,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="246" ht="15.75" customHeight="1">
+    <row r="246" spans="1:86" ht="15.75" customHeight="1">
       <c r="A246" s="4" t="s">
         <v>332</v>
       </c>
@@ -53761,7 +53777,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="247" ht="15.75" customHeight="1">
+    <row r="247" spans="1:86" ht="15.75" customHeight="1">
       <c r="A247" s="4" t="s">
         <v>333</v>
       </c>
@@ -53971,7 +53987,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="248" ht="15.75" customHeight="1">
+    <row r="248" spans="1:86" ht="15.75" customHeight="1">
       <c r="A248" s="4" t="s">
         <v>334</v>
       </c>
@@ -54181,7 +54197,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="249" ht="15.75" customHeight="1">
+    <row r="249" spans="1:86" ht="15.75" customHeight="1">
       <c r="A249" s="4" t="s">
         <v>335</v>
       </c>
@@ -54391,7 +54407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="250" ht="15.75" customHeight="1">
+    <row r="250" spans="1:86" ht="15.75" customHeight="1">
       <c r="A250" s="4" t="s">
         <v>336</v>
       </c>
@@ -54601,7 +54617,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="251" ht="15.75" customHeight="1">
+    <row r="251" spans="1:86" ht="15.75" customHeight="1">
       <c r="A251" s="4" t="s">
         <v>337</v>
       </c>
@@ -54811,7 +54827,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="252" ht="15.75" customHeight="1">
+    <row r="252" spans="1:86" ht="15.75" customHeight="1">
       <c r="A252" s="4" t="s">
         <v>338</v>
       </c>
@@ -55027,7 +55043,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
+    <row r="253" spans="1:86" ht="15.75" customHeight="1">
       <c r="A253" s="4" t="s">
         <v>339</v>
       </c>
@@ -55237,7 +55253,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="254" ht="15.75" customHeight="1">
+    <row r="254" spans="1:86" ht="15.75" customHeight="1">
       <c r="A254" s="4" t="s">
         <v>340</v>
       </c>
@@ -55447,7 +55463,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="255" ht="15.75" customHeight="1">
+    <row r="255" spans="1:86" ht="15.75" customHeight="1">
       <c r="A255" s="4" t="s">
         <v>341</v>
       </c>
@@ -55657,7 +55673,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="256" ht="15.75" customHeight="1">
+    <row r="256" spans="1:86" ht="15.75" customHeight="1">
       <c r="A256" s="4" t="s">
         <v>342</v>
       </c>
@@ -55869,7 +55885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="257" ht="15.75" customHeight="1">
+    <row r="257" spans="1:86" ht="15.75" customHeight="1">
       <c r="A257" s="4" t="s">
         <v>343</v>
       </c>
@@ -56083,7 +56099,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="258" ht="15.75" customHeight="1">
+    <row r="258" spans="1:86" ht="15.75" customHeight="1">
       <c r="A258" s="4" t="s">
         <v>344</v>
       </c>
@@ -56295,7 +56311,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="259" ht="15.75" customHeight="1">
+    <row r="259" spans="1:86" ht="15.75" customHeight="1">
       <c r="A259" s="4" t="s">
         <v>345</v>
       </c>
@@ -56507,7 +56523,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="260" ht="15.75" customHeight="1">
+    <row r="260" spans="1:86" ht="15.75" customHeight="1">
       <c r="A260" s="4" t="s">
         <v>346</v>
       </c>
@@ -56717,7 +56733,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="261" ht="15.75" customHeight="1">
+    <row r="261" spans="1:86" ht="15.75" customHeight="1">
       <c r="A261" s="4" t="s">
         <v>347</v>
       </c>
@@ -56927,7 +56943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="262" ht="15.75" customHeight="1">
+    <row r="262" spans="1:86" ht="15.75" customHeight="1">
       <c r="A262" s="4" t="s">
         <v>348</v>
       </c>
@@ -57139,7 +57155,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="263" ht="15.75" customHeight="1">
+    <row r="263" spans="1:86" ht="15.75" customHeight="1">
       <c r="A263" s="4" t="s">
         <v>349</v>
       </c>
@@ -57349,7 +57365,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="264" ht="15.75" customHeight="1">
+    <row r="264" spans="1:86" ht="15.75" customHeight="1">
       <c r="A264" s="4" t="s">
         <v>350</v>
       </c>
@@ -57563,7 +57579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="265" ht="15.75" customHeight="1">
+    <row r="265" spans="1:86" ht="15.75" customHeight="1">
       <c r="A265" s="4" t="s">
         <v>351</v>
       </c>
@@ -57773,7 +57789,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="266" ht="15.75" customHeight="1">
+    <row r="266" spans="1:86" ht="15.75" customHeight="1">
       <c r="A266" s="4" t="s">
         <v>352</v>
       </c>
@@ -57987,7 +58003,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="267" ht="15.75" customHeight="1">
+    <row r="267" spans="1:86" ht="15.75" customHeight="1">
       <c r="A267" s="4" t="s">
         <v>353</v>
       </c>
@@ -58197,7 +58213,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="268" ht="15.75" customHeight="1">
+    <row r="268" spans="1:86" ht="15.75" customHeight="1">
       <c r="A268" s="4" t="s">
         <v>354</v>
       </c>
@@ -58407,7 +58423,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="269" ht="15.75" customHeight="1">
+    <row r="269" spans="1:86" ht="15.75" customHeight="1">
       <c r="A269" s="4" t="s">
         <v>355</v>
       </c>
@@ -58619,7 +58635,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="270" ht="15.75" customHeight="1">
+    <row r="270" spans="1:86" ht="15.75" customHeight="1">
       <c r="A270" s="4" t="s">
         <v>356</v>
       </c>
@@ -58829,7 +58845,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="271" ht="15.75" customHeight="1">
+    <row r="271" spans="1:86" ht="15.75" customHeight="1">
       <c r="A271" s="4" t="s">
         <v>357</v>
       </c>
@@ -59039,7 +59055,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="272" ht="15.75" customHeight="1">
+    <row r="272" spans="1:86" ht="15.75" customHeight="1">
       <c r="A272" s="4" t="s">
         <v>358</v>
       </c>
@@ -59249,7 +59265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="273" ht="15.75" customHeight="1">
+    <row r="273" spans="1:86" ht="15.75" customHeight="1">
       <c r="A273" s="4" t="s">
         <v>359</v>
       </c>
@@ -59459,7 +59475,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="274" ht="15.75" customHeight="1">
+    <row r="274" spans="1:86" ht="15.75" customHeight="1">
       <c r="A274" s="4" t="s">
         <v>360</v>
       </c>
@@ -59669,7 +59685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="275" ht="15.75" customHeight="1">
+    <row r="275" spans="1:86" ht="15.75" customHeight="1">
       <c r="A275" s="4" t="s">
         <v>361</v>
       </c>
@@ -59879,7 +59895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="276" ht="15.75" customHeight="1">
+    <row r="276" spans="1:86" ht="15.75" customHeight="1">
       <c r="A276" s="4" t="s">
         <v>362</v>
       </c>
@@ -60089,7 +60105,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="277" ht="15.75" customHeight="1">
+    <row r="277" spans="1:86" ht="15.75" customHeight="1">
       <c r="A277" s="4" t="s">
         <v>363</v>
       </c>
@@ -60303,7 +60319,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="278" ht="15.75" customHeight="1">
+    <row r="278" spans="1:86" ht="15.75" customHeight="1">
       <c r="A278" s="4" t="s">
         <v>364</v>
       </c>
@@ -60513,7 +60529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="279" ht="15.75" customHeight="1">
+    <row r="279" spans="1:86" ht="15.75" customHeight="1">
       <c r="A279" s="4" t="s">
         <v>365</v>
       </c>
@@ -60723,7 +60739,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="280" ht="15.75" customHeight="1">
+    <row r="280" spans="1:86" ht="15.75" customHeight="1">
       <c r="A280" s="4" t="s">
         <v>366</v>
       </c>
@@ -60933,7 +60949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="281" ht="15.75" customHeight="1">
+    <row r="281" spans="1:86" ht="15.75" customHeight="1">
       <c r="A281" s="4" t="s">
         <v>367</v>
       </c>
@@ -61143,7 +61159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="282" ht="15.75" customHeight="1">
+    <row r="282" spans="1:86" ht="15.75" customHeight="1">
       <c r="A282" s="4" t="s">
         <v>368</v>
       </c>
@@ -61353,7 +61369,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="283" ht="15.75" customHeight="1">
+    <row r="283" spans="1:86" ht="15.75" customHeight="1">
       <c r="A283" s="4" t="s">
         <v>369</v>
       </c>
@@ -61563,7 +61579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="284" ht="15.75" customHeight="1">
+    <row r="284" spans="1:86" ht="15.75" customHeight="1">
       <c r="A284" s="4" t="s">
         <v>370</v>
       </c>
@@ -61773,7 +61789,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="285" ht="15.75" customHeight="1">
+    <row r="285" spans="1:86" ht="15.75" customHeight="1">
       <c r="A285" s="4" t="s">
         <v>371</v>
       </c>
@@ -61985,7 +62001,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="286" ht="15.75" customHeight="1">
+    <row r="286" spans="1:86" ht="15.75" customHeight="1">
       <c r="A286" s="4" t="s">
         <v>372</v>
       </c>
@@ -62195,7 +62211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="287" ht="15.75" customHeight="1">
+    <row r="287" spans="1:86" ht="15.75" customHeight="1">
       <c r="A287" s="4" t="s">
         <v>373</v>
       </c>
@@ -62405,7 +62421,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="288" ht="15.75" customHeight="1">
+    <row r="288" spans="1:86" ht="15.75" customHeight="1">
       <c r="A288" s="4" t="s">
         <v>374</v>
       </c>
@@ -62615,7 +62631,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="289" ht="15.75" customHeight="1">
+    <row r="289" spans="1:86" ht="15.75" customHeight="1">
       <c r="A289" s="4" t="s">
         <v>375</v>
       </c>
@@ -62825,7 +62841,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="290" ht="15.75" customHeight="1">
+    <row r="290" spans="1:86" ht="15.75" customHeight="1">
       <c r="A290" s="4" t="s">
         <v>376</v>
       </c>
@@ -63035,7 +63051,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="291" ht="15.75" customHeight="1">
+    <row r="291" spans="1:86" ht="15.75" customHeight="1">
       <c r="A291" s="4" t="s">
         <v>377</v>
       </c>
@@ -63245,7 +63261,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="292" ht="15.75" customHeight="1">
+    <row r="292" spans="1:86" ht="15.75" customHeight="1">
       <c r="A292" s="4" t="s">
         <v>378</v>
       </c>
@@ -63455,7 +63471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="293" ht="15.75" customHeight="1">
+    <row r="293" spans="1:86" ht="15.75" customHeight="1">
       <c r="A293" s="4" t="s">
         <v>379</v>
       </c>
@@ -63665,7 +63681,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="294" ht="15.75" customHeight="1">
+    <row r="294" spans="1:86" ht="15.75" customHeight="1">
       <c r="A294" s="4" t="s">
         <v>380</v>
       </c>
@@ -63875,7 +63891,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="295" ht="15.75" customHeight="1">
+    <row r="295" spans="1:86" ht="15.75" customHeight="1">
       <c r="A295" s="4" t="s">
         <v>381</v>
       </c>
@@ -64089,7 +64105,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="296" ht="15.75" customHeight="1">
+    <row r="296" spans="1:86" ht="15.75" customHeight="1">
       <c r="A296" s="4" t="s">
         <v>382</v>
       </c>
@@ -64299,7 +64315,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="297" ht="15.75" customHeight="1">
+    <row r="297" spans="1:86" ht="15.75" customHeight="1">
       <c r="A297" s="4" t="s">
         <v>383</v>
       </c>
@@ -64509,7 +64525,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="298" ht="15.75" customHeight="1">
+    <row r="298" spans="1:86" ht="15.75" customHeight="1">
       <c r="A298" s="4" t="s">
         <v>384</v>
       </c>
@@ -64719,7 +64735,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="299" ht="15.75" customHeight="1">
+    <row r="299" spans="1:86" ht="15.75" customHeight="1">
       <c r="A299" s="4" t="s">
         <v>385</v>
       </c>
@@ -64929,7 +64945,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="300" ht="15.75" customHeight="1">
+    <row r="300" spans="1:86" ht="15.75" customHeight="1">
       <c r="A300" s="4" t="s">
         <v>386</v>
       </c>
@@ -65139,7 +65155,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="301" ht="15.75" customHeight="1">
+    <row r="301" spans="1:86" ht="15.75" customHeight="1">
       <c r="A301" s="4" t="s">
         <v>387</v>
       </c>
@@ -65349,7 +65365,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="302" ht="15.75" customHeight="1">
+    <row r="302" spans="1:86" ht="15.75" customHeight="1">
       <c r="A302" s="4" t="s">
         <v>388</v>
       </c>
@@ -65559,7 +65575,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="303" ht="15.75" customHeight="1">
+    <row r="303" spans="1:86" ht="15.75" customHeight="1">
       <c r="A303" s="4" t="s">
         <v>389</v>
       </c>
@@ -65769,7 +65785,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="304" ht="15.75" customHeight="1">
+    <row r="304" spans="1:86" ht="15.75" customHeight="1">
       <c r="A304" s="4" t="s">
         <v>390</v>
       </c>
@@ -65979,7 +65995,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="305" ht="15.75" customHeight="1">
+    <row r="305" spans="1:86" ht="15.75" customHeight="1">
       <c r="A305" s="4" t="s">
         <v>82</v>
       </c>
@@ -66189,7 +66205,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="306" ht="15.75" customHeight="1">
+    <row r="306" spans="1:86" ht="15.75" customHeight="1">
       <c r="A306" s="4" t="s">
         <v>391</v>
       </c>
@@ -66399,7 +66415,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="307" ht="15.75" customHeight="1">
+    <row r="307" spans="1:86" ht="15.75" customHeight="1">
       <c r="A307" s="4" t="s">
         <v>392</v>
       </c>
@@ -66609,7 +66625,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="308" ht="15.75" customHeight="1">
+    <row r="308" spans="1:86" ht="15.75" customHeight="1">
       <c r="A308" s="4" t="s">
         <v>393</v>
       </c>
@@ -66819,7 +66835,7 @@
       <c r="CG308" s="5"/>
       <c r="CH308" s="5"/>
     </row>
-    <row r="309" ht="15.75" customHeight="1">
+    <row r="309" spans="1:86" ht="15.75" customHeight="1">
       <c r="A309" s="4" t="s">
         <v>394</v>
       </c>
@@ -67029,7 +67045,7 @@
       <c r="CG309" s="5"/>
       <c r="CH309" s="5"/>
     </row>
-    <row r="310" ht="15.75" customHeight="1">
+    <row r="310" spans="1:86" ht="15.75" customHeight="1">
       <c r="A310" s="4" t="s">
         <v>395</v>
       </c>
@@ -67237,7 +67253,7 @@
       <c r="CG310" s="5"/>
       <c r="CH310" s="5"/>
     </row>
-    <row r="311" ht="15.75" customHeight="1">
+    <row r="311" spans="1:86" ht="15.75" customHeight="1">
       <c r="A311" s="4" t="s">
         <v>396</v>
       </c>
@@ -67447,7 +67463,7 @@
       <c r="CG311" s="5"/>
       <c r="CH311" s="5"/>
     </row>
-    <row r="312" ht="15.75" customHeight="1">
+    <row r="312" spans="1:86" ht="15.75" customHeight="1">
       <c r="A312" s="4" t="s">
         <v>397</v>
       </c>
@@ -67653,7 +67669,7 @@
       <c r="CG312" s="5"/>
       <c r="CH312" s="5"/>
     </row>
-    <row r="313" ht="15.75" customHeight="1">
+    <row r="313" spans="1:86" ht="15.75" customHeight="1">
       <c r="A313" s="4" t="s">
         <v>398</v>
       </c>
@@ -67861,7 +67877,7 @@
       <c r="CG313" s="5"/>
       <c r="CH313" s="5"/>
     </row>
-    <row r="314" ht="15.75" customHeight="1">
+    <row r="314" spans="1:86" ht="15.75" customHeight="1">
       <c r="A314" s="4" t="s">
         <v>399</v>
       </c>
@@ -68067,7 +68083,7 @@
       <c r="CG314" s="5"/>
       <c r="CH314" s="5"/>
     </row>
-    <row r="315" ht="15.75" customHeight="1">
+    <row r="315" spans="1:86" ht="15.75" customHeight="1">
       <c r="A315" s="4" t="s">
         <v>400</v>
       </c>
@@ -68273,7 +68289,7 @@
       <c r="CG315" s="5"/>
       <c r="CH315" s="5"/>
     </row>
-    <row r="316" ht="15.75" customHeight="1">
+    <row r="316" spans="1:86" ht="15.75" customHeight="1">
       <c r="A316" s="4" t="s">
         <v>401</v>
       </c>
@@ -68479,7 +68495,7 @@
       <c r="CG316" s="5"/>
       <c r="CH316" s="5"/>
     </row>
-    <row r="317" ht="15.75" customHeight="1">
+    <row r="317" spans="1:86" ht="15.75" customHeight="1">
       <c r="A317" s="4" t="s">
         <v>402</v>
       </c>
@@ -68687,7 +68703,7 @@
       <c r="CG317" s="5"/>
       <c r="CH317" s="5"/>
     </row>
-    <row r="318" ht="15.75" customHeight="1">
+    <row r="318" spans="1:86" ht="15.75" customHeight="1">
       <c r="A318" s="4" t="s">
         <v>403</v>
       </c>
@@ -68897,7 +68913,7 @@
       <c r="CG318" s="5"/>
       <c r="CH318" s="5"/>
     </row>
-    <row r="319" ht="15.75" customHeight="1">
+    <row r="319" spans="1:86" ht="15.75" customHeight="1">
       <c r="A319" s="4" t="s">
         <v>404</v>
       </c>
@@ -69103,7 +69119,7 @@
       <c r="CG319" s="5"/>
       <c r="CH319" s="5"/>
     </row>
-    <row r="320" ht="15.75" customHeight="1">
+    <row r="320" spans="1:86" ht="15.75" customHeight="1">
       <c r="A320" s="4" t="s">
         <v>405</v>
       </c>
@@ -69307,7 +69323,7 @@
       <c r="CG320" s="5"/>
       <c r="CH320" s="5"/>
     </row>
-    <row r="321" ht="15.75" customHeight="1">
+    <row r="321" spans="1:86" ht="15.75" customHeight="1">
       <c r="A321" s="4" t="s">
         <v>406</v>
       </c>
@@ -69513,7 +69529,7 @@
       <c r="CG321" s="5"/>
       <c r="CH321" s="5"/>
     </row>
-    <row r="322" ht="15.75" customHeight="1">
+    <row r="322" spans="1:86" ht="15.75" customHeight="1">
       <c r="A322" s="4" t="s">
         <v>407</v>
       </c>
@@ -69719,20 +69735,20 @@
       <c r="CG322" s="5"/>
       <c r="CH322" s="5"/>
     </row>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="323" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="324" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="325" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="326" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="327" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="328" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="329" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="330" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="331" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="332" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="333" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="334" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="335" spans="1:86" ht="15.75" customHeight="1"/>
+    <row r="336" spans="1:86" ht="15.75" customHeight="1"/>
     <row r="337" ht="15.75" customHeight="1"/>
     <row r="338" ht="15.75" customHeight="1"/>
     <row r="339" ht="15.75" customHeight="1"/>
@@ -70399,18 +70415,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="B2:CH322">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:CH322">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>